<commit_message>
fix routing bug when testing
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanggor\Documents\Wanggor\Project\pelabuhan\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B90B46-3D3A-476D-A2CF-FAC781F886E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F135218-47C1-49EB-8540-06E8A07314AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Biaya_Jarak_Teus" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="384">
   <si>
     <t>Ilwaki</t>
   </si>
@@ -12429,8 +12429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DEB37C-F1F6-4802-96BB-B6E3BD9E329B}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D90" sqref="A2:D90"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13740,10 +13740,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D59823-B98E-469E-B8CC-629204B9A535}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -13777,14 +13777,14 @@
       <c r="A2" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>46</v>
+      <c r="B2" s="26" t="s">
+        <v>76</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="E2" s="25">
         <v>47</v>
@@ -13793,21 +13793,1500 @@
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" ht="15.6">
+    <row r="3" spans="1:10">
       <c r="A3" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>76</v>
+      <c r="B3" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22">
+        <v>9</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34">
+        <v>9</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37">
+        <v>9</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48">
+        <v>9</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <v>9</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57">
+        <v>8</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C58">
+        <v>7</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59">
+        <v>7</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E62" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63">
+        <v>8</v>
+      </c>
+      <c r="D63" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E63" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65">
+        <v>7</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66">
+        <v>9</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E66" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="B67" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="25">
-        <v>48</v>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E67" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B68" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68">
+        <v>9</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C69">
+        <v>9</v>
+      </c>
+      <c r="D69" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E69" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70">
+        <v>9</v>
+      </c>
+      <c r="D70" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71">
+        <v>8</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E71" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E72" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73">
+        <v>8</v>
+      </c>
+      <c r="D73" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74">
+        <v>8</v>
+      </c>
+      <c r="D74" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E74" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B75" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75">
+        <v>6</v>
+      </c>
+      <c r="D75" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E75" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>6</v>
+      </c>
+      <c r="D76" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="B77" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E77" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <v>8</v>
+      </c>
+      <c r="D78" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E78" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B79" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79">
+        <v>6</v>
+      </c>
+      <c r="D79" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E79" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B80" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C80">
+        <v>4</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="B81" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+      <c r="D81" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E81" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="B82" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C82">
+        <v>6</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="B83" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+      <c r="D83" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B84" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C84">
+        <v>9</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85">
+        <v>6</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E85" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86">
+        <v>5</v>
+      </c>
+      <c r="D86" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E86" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B87" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C87">
+        <v>7</v>
+      </c>
+      <c r="D87" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E87" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B88" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C88">
+        <v>8</v>
+      </c>
+      <c r="D88" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E88" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="B89" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C89">
+        <v>8</v>
+      </c>
+      <c r="D89" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E89" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B90" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C90">
+        <v>6</v>
+      </c>
+      <c r="D90" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="25">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -23305,8 +24784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC93771-8FE0-4248-8EEE-4AB295A47998}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -23637,8 +25116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851089AA-D5A7-4C66-A791-D07CFCF5E603}">
   <dimension ref="A1:BZ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -24896,7 +26375,7 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -25132,7 +26611,7 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -25368,7 +26847,7 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -25604,7 +27083,7 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="X9">
         <v>0</v>

</xml_diff>

<commit_message>
fix route for PELNI
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanggor\Documents\Wanggor\Project\pelabuhan\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D6CBEA-13DB-4A42-9AED-DAFE70DD6C88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAE6850-5E69-45E8-862D-237AA1EA872E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="9" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="10" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Biaya_Jarak_Teus" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="ports" sheetId="8" r:id="rId8"/>
     <sheet name="port_loc" sheetId="11" r:id="rId9"/>
     <sheet name="Rute" sheetId="17" r:id="rId10"/>
+    <sheet name="TL_PL_RUTE" sheetId="18" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="309">
   <si>
     <t>Ilwaki</t>
   </si>
@@ -975,6 +976,12 @@
   <si>
     <t>1°19'52.2"S</t>
   </si>
+  <si>
+    <t>Daftar Rute Tol Laut</t>
+  </si>
+  <si>
+    <t>Daftar Rute Pelni</t>
+  </si>
 </sst>
 </file>
 
@@ -1293,7 +1300,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1353,6 +1360,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1365,6 +1374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -12227,8 +12237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2313015A-8265-4AFC-B00C-44D39E89E7D7}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12254,10 +12264,10 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C2" s="31" t="s">
@@ -12268,8 +12278,8 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="40"/>
-      <c r="B3" s="37"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="31" t="s">
         <v>303</v>
       </c>
@@ -12278,8 +12288,8 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="40"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="31" t="s">
         <v>306</v>
       </c>
@@ -12288,8 +12298,8 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="40"/>
-      <c r="B5" s="38"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="28" t="s">
         <v>130</v>
       </c>
@@ -12304,6 +12314,159 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E87E26-6ABF-4B30-8964-7B51A59EDE4F}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="37"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="43"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="43"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="43"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="43"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="43"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="43"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="43"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="43"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="43"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="43"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="F14" s="43"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="F15" s="43"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="F16" s="43"/>
+    </row>
+    <row r="17" spans="6:6">
+      <c r="F17" s="43"/>
+    </row>
+    <row r="18" spans="6:6">
+      <c r="F18" s="43"/>
+    </row>
+    <row r="19" spans="6:6">
+      <c r="F19" s="43"/>
+    </row>
+    <row r="20" spans="6:6">
+      <c r="F20" s="43"/>
+    </row>
+    <row r="21" spans="6:6">
+      <c r="F21" s="43"/>
+    </row>
+    <row r="22" spans="6:6">
+      <c r="F22" s="43"/>
+    </row>
+    <row r="23" spans="6:6">
+      <c r="F23" s="43"/>
+    </row>
+    <row r="24" spans="6:6">
+      <c r="F24" s="43"/>
+    </row>
+    <row r="25" spans="6:6">
+      <c r="F25" s="43"/>
+    </row>
+    <row r="26" spans="6:6">
+      <c r="F26" s="43"/>
+    </row>
+    <row r="27" spans="6:6">
+      <c r="F27" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -32906,7 +33069,7 @@
   <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>